<commit_message>
codigo 100 pocento funcional, falta add editar livro, add na proixma att
</commit_message>
<xml_diff>
--- a/teste/pro/livros.xlsx
+++ b/teste/pro/livros.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -423,41 +423,521 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>1234567890</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>O Poder do Pensamento</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Editora X</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>João Silva</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Uma história inspiradora</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Detalhes adicionais...</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>3</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1234567890</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>O Poder do Pensamento</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Editora X</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>João Silva</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Uma história inspiradora</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Detalhes adicionais...</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1234567890</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>O Poder do Pensamento</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Editora X</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>João Silva</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Uma história inspiradora</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Detalhes adicionais...</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>5</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>10</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>naruto</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>lertras</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>brascuabs</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>livreo de tesrte</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>6</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1234567890</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>O Poder do Pensamento</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Editora X</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>João Silva</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Uma história inspiradora</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Detalhes adicionais...</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>7</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1234567890</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>O Poder do Pensamento</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Editora X</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>João Silva</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Uma história inspiradora</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Detalhes adicionais...</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>8</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>1234567890</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>O Poder do Pensamento</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Editora X</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>João Silva</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Uma história inspiradora</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Detalhes adicionais...</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>9</v>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>brascubas</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>nova</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>brascubas</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>letras</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
         <is>
           <t>machado</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>autor escreve sua vidada desade a morte ate o nascimento.</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>sim</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>livro : descrito na seção 10 esta na apa norte aramrio 2 sub pasta 4.</t>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>mahcao escrevs sua vida ja morto</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>nao</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>10</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>11</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1234567890</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>O Poder do Pensamento</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Editora X</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>João Silva</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Uma história inspiradora</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Detalhes adicionais...</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>12</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1234567890</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>O Poder do Pensamento</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Editora X</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>João Silva</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Uma história inspiradora</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Detalhes adicionais...</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>13</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>111</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>111</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>letras</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>livros de teste 111</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>campo para detalçhes extrs sobre o livro</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>14</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>111</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>dois</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>letras</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>bras</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>brassss</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>naso</t>
         </is>
       </c>
     </row>

</xml_diff>